<commit_message>
added the updated UI
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -397,19 +397,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>z@gmail.com</v>
+        <v>abibangbrandon855@gmail.com</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>abibangbrandon86655@gmail.com</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>abibangbrandon87755@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactored the success, error and inde.ejs styling
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -417,9 +417,34 @@
         <v>abibangbrandon87755@gmail.com</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>abibangbranfffdon855@gmail.com</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>rrrr@gmail.com</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>a@gmail.com</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>bbb@gmail.com</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>ggffg@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:A3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:A8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>